<commit_message>
Manuell kjøring av program
</commit_message>
<xml_diff>
--- a/output/Lagserien 2023 1-2. div.xlsx
+++ b/output/Lagserien 2023 1-2. div.xlsx
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>24010</v>
+        <v>24015</v>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
@@ -852,11 +852,11 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>(30/12)</t>
+          <t>(30/13)</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>21109</v>
+        <v>21215</v>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
@@ -936,11 +936,11 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>(29/12)</t>
+          <t>(29/11)</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>17704</v>
+        <v>18044</v>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
@@ -5026,18 +5026,18 @@
         <v>1999</v>
       </c>
       <c r="O91" s="15" t="n">
-        <v>50.71</v>
+        <v>50.61</v>
       </c>
       <c r="P91" s="7" t="n">
-        <v>748</v>
+        <v>753</v>
       </c>
       <c r="Q91" s="7" t="inlineStr">
         <is>
-          <t>Moelv</t>
+          <t>Paris/FRA</t>
         </is>
       </c>
       <c r="R91" s="16" t="n">
-        <v>21.05</v>
+        <v>15.07</v>
       </c>
       <c r="T91" s="5" t="n"/>
     </row>
@@ -5381,7 +5381,7 @@
         </is>
       </c>
       <c r="P98" s="20" t="n">
-        <v>11656</v>
+        <v>11661</v>
       </c>
       <c r="T98" s="5" t="n"/>
     </row>
@@ -5421,7 +5421,7 @@
         </is>
       </c>
       <c r="P100" s="20" t="n">
-        <v>24010</v>
+        <v>24015</v>
       </c>
       <c r="T100" s="5" t="n"/>
     </row>
@@ -11891,25 +11891,25 @@
       </c>
       <c r="M250" s="7" t="inlineStr">
         <is>
-          <t>Aksel Wormdahl</t>
+          <t>Sverre Ranes Olstad</t>
         </is>
       </c>
       <c r="N250" s="7" t="n">
         <v>2006</v>
       </c>
       <c r="O250" s="15" t="n">
-        <v>2.8</v>
+        <v>2.82</v>
       </c>
       <c r="P250" s="7" t="n">
-        <v>561</v>
+        <v>572</v>
       </c>
       <c r="Q250" s="7" t="inlineStr">
         <is>
-          <t>Ranheim</t>
+          <t>Stjørdal</t>
         </is>
       </c>
       <c r="R250" s="16" t="n">
-        <v>29.01</v>
+        <v>8.06</v>
       </c>
       <c r="T250" s="5" t="n"/>
     </row>
@@ -11949,17 +11949,17 @@
       </c>
       <c r="M251" s="7" t="inlineStr">
         <is>
-          <t>Emil Vestre</t>
+          <t>Aksel Wormdahl</t>
         </is>
       </c>
       <c r="N251" s="7" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="O251" s="15" t="n">
-        <v>2.79</v>
+        <v>2.8</v>
       </c>
       <c r="P251" s="7" t="n">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="Q251" s="7" t="inlineStr">
         <is>
@@ -12007,17 +12007,17 @@
       </c>
       <c r="M252" s="7" t="inlineStr">
         <is>
-          <t>Tomas Digernes Heltne</t>
+          <t>Emil Vestre</t>
         </is>
       </c>
       <c r="N252" s="7" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="O252" s="15" t="n">
-        <v>2.64</v>
+        <v>2.79</v>
       </c>
       <c r="P252" s="7" t="n">
-        <v>466</v>
+        <v>555</v>
       </c>
       <c r="Q252" s="7" t="inlineStr">
         <is>
@@ -12079,7 +12079,7 @@
         </is>
       </c>
       <c r="P254" s="20" t="n">
-        <v>9965</v>
+        <v>10071</v>
       </c>
       <c r="T254" s="5" t="n"/>
     </row>
@@ -12119,7 +12119,7 @@
         </is>
       </c>
       <c r="P256" s="20" t="n">
-        <v>21109</v>
+        <v>21215</v>
       </c>
       <c r="T256" s="5" t="n"/>
     </row>
@@ -12143,7 +12143,7 @@
         </is>
       </c>
       <c r="M258" s="20" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T258" s="5" t="n"/>
     </row>
@@ -14565,25 +14565,25 @@
       </c>
       <c r="C322" s="7" t="inlineStr">
         <is>
-          <t>Sondre Høylo Trefall</t>
+          <t>Eirik Reigstad</t>
         </is>
       </c>
       <c r="D322" s="7" t="n">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E322" s="15" t="n">
-        <v>13.27</v>
+        <v>11.95</v>
       </c>
       <c r="F322" s="7" t="n">
-        <v>375</v>
+        <v>621</v>
       </c>
       <c r="G322" s="7" t="inlineStr">
         <is>
-          <t>Fana</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="H322" s="16" t="n">
-        <v>4.06</v>
+        <v>5.07</v>
       </c>
       <c r="J322" s="5" t="n"/>
       <c r="L322" s="14" t="inlineStr">
@@ -15380,7 +15380,7 @@
         </is>
       </c>
       <c r="F337" s="20" t="n">
-        <v>9369</v>
+        <v>9615</v>
       </c>
       <c r="J337" s="5" t="n"/>
       <c r="L337" s="19" t="inlineStr">
@@ -15796,7 +15796,7 @@
     <row r="347" ht="13" customHeight="1">
       <c r="B347" s="14" t="inlineStr">
         <is>
-          <t>200m</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="C347" s="7" t="inlineStr">
@@ -15808,18 +15808,18 @@
         <v>2007</v>
       </c>
       <c r="E347" s="15" t="n">
-        <v>24.86</v>
+        <v>7.67</v>
       </c>
       <c r="F347" s="7" t="n">
-        <v>568</v>
+        <v>600</v>
       </c>
       <c r="G347" s="7" t="inlineStr">
         <is>
-          <t>Rosendal</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="H347" s="16" t="n">
-        <v>28.05</v>
+        <v>5.07</v>
       </c>
       <c r="J347" s="5" t="n"/>
       <c r="L347" s="14" t="inlineStr">
@@ -15856,7 +15856,7 @@
     <row r="348" ht="13" customHeight="1">
       <c r="B348" s="14" t="inlineStr">
         <is>
-          <t>60m</t>
+          <t>200m</t>
         </is>
       </c>
       <c r="C348" s="7" t="inlineStr">
@@ -15868,18 +15868,18 @@
         <v>2007</v>
       </c>
       <c r="E348" s="15" t="n">
-        <v>7.82</v>
+        <v>24.86</v>
       </c>
       <c r="F348" s="7" t="n">
-        <v>551</v>
+        <v>568</v>
       </c>
       <c r="G348" s="7" t="inlineStr">
         <is>
-          <t>Leikvang</t>
+          <t>Rosendal</t>
         </is>
       </c>
       <c r="H348" s="16" t="n">
-        <v>11.02</v>
+        <v>28.05</v>
       </c>
       <c r="J348" s="5" t="n"/>
       <c r="L348" s="14" t="inlineStr">
@@ -15916,7 +15916,7 @@
     <row r="349" ht="13" customHeight="1">
       <c r="B349" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>5000m</t>
         </is>
       </c>
       <c r="C349" s="7" t="inlineStr">
@@ -15929,11 +15929,11 @@
       </c>
       <c r="E349" s="17" t="inlineStr">
         <is>
-          <t>9,46,87</t>
+          <t>16,52,24</t>
         </is>
       </c>
       <c r="F349" s="7" t="n">
-        <v>529</v>
+        <v>548</v>
       </c>
       <c r="G349" s="7" t="inlineStr">
         <is>
@@ -15941,7 +15941,7 @@
         </is>
       </c>
       <c r="H349" s="16" t="n">
-        <v>26.06</v>
+        <v>5.07</v>
       </c>
       <c r="J349" s="5" t="n"/>
       <c r="L349" s="14" t="inlineStr">
@@ -15978,30 +15978,32 @@
     <row r="350" ht="13" customHeight="1">
       <c r="B350" s="14" t="inlineStr">
         <is>
-          <t>Høyde u.t</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="C350" s="7" t="inlineStr">
         <is>
-          <t>Magnus Reigstad</t>
+          <t>Daniel Bruvik</t>
         </is>
       </c>
       <c r="D350" s="7" t="n">
-        <v>2003</v>
-      </c>
-      <c r="E350" s="15" t="n">
-        <v>1.36</v>
+        <v>1996</v>
+      </c>
+      <c r="E350" s="17" t="inlineStr">
+        <is>
+          <t>9,46,87</t>
+        </is>
       </c>
       <c r="F350" s="7" t="n">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="G350" s="7" t="inlineStr">
         <is>
-          <t>Osterøy</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="H350" s="16" t="n">
-        <v>16.01</v>
+        <v>26.06</v>
       </c>
       <c r="J350" s="5" t="n"/>
       <c r="L350" s="14" t="inlineStr">
@@ -16043,25 +16045,25 @@
       </c>
       <c r="C351" s="7" t="inlineStr">
         <is>
-          <t>Eirik Reigstad</t>
+          <t>Magnus Reigstad</t>
         </is>
       </c>
       <c r="D351" s="7" t="n">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="E351" s="15" t="n">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="F351" s="7" t="n">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="G351" s="7" t="inlineStr">
         <is>
-          <t>Leikvang</t>
+          <t>Osterøy</t>
         </is>
       </c>
       <c r="H351" s="16" t="n">
-        <v>10.02</v>
+        <v>16.01</v>
       </c>
       <c r="J351" s="5" t="n"/>
       <c r="L351" s="14" t="inlineStr">
@@ -16320,7 +16322,7 @@
         </is>
       </c>
       <c r="F358" s="20" t="n">
-        <v>8335</v>
+        <v>8429</v>
       </c>
       <c r="J358" s="5" t="n"/>
       <c r="L358" s="19" t="inlineStr">
@@ -16360,7 +16362,7 @@
         </is>
       </c>
       <c r="F360" s="20" t="n">
-        <v>17704</v>
+        <v>18044</v>
       </c>
       <c r="J360" s="5" t="n"/>
       <c r="L360" s="19" t="inlineStr">
@@ -16392,7 +16394,7 @@
         </is>
       </c>
       <c r="C362" s="20" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J362" s="5" t="n"/>
       <c r="L362" s="19" t="inlineStr">
@@ -16433,20 +16435,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="P262:Q263"/>
-    <mergeCell ref="F210:G211"/>
     <mergeCell ref="F2:G3"/>
+    <mergeCell ref="P2:Q3"/>
     <mergeCell ref="F54:G55"/>
-    <mergeCell ref="P314:Q315"/>
-    <mergeCell ref="F314:G315"/>
     <mergeCell ref="P54:Q55"/>
-    <mergeCell ref="P2:Q3"/>
     <mergeCell ref="F106:G107"/>
+    <mergeCell ref="P106:Q107"/>
     <mergeCell ref="F158:G159"/>
     <mergeCell ref="P158:Q159"/>
+    <mergeCell ref="F210:G211"/>
     <mergeCell ref="P210:Q211"/>
-    <mergeCell ref="P106:Q107"/>
     <mergeCell ref="F262:G263"/>
+    <mergeCell ref="P262:Q263"/>
+    <mergeCell ref="F314:G315"/>
+    <mergeCell ref="P314:Q315"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -16541,11 +16543,11 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>(25/12)</t>
+          <t>(25/11)</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>16750</v>
+        <v>16769</v>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
@@ -16769,7 +16771,7 @@
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>15059</v>
+        <v>15099</v>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
@@ -18449,18 +18451,18 @@
         <v>2009</v>
       </c>
       <c r="O34" s="15" t="n">
-        <v>7.9</v>
+        <v>7.84</v>
       </c>
       <c r="P34" s="7" t="n">
-        <v>526</v>
+        <v>545</v>
       </c>
       <c r="Q34" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Søgne</t>
         </is>
       </c>
       <c r="R34" s="16" t="n">
-        <v>17.06</v>
+        <v>23.05</v>
       </c>
       <c r="T34" s="5" t="n"/>
     </row>
@@ -18502,7 +18504,7 @@
       </c>
       <c r="M35" s="7" t="inlineStr">
         <is>
-          <t>Olai Stav Grosvold</t>
+          <t>Olai Stav Graasvoll</t>
         </is>
       </c>
       <c r="N35" s="7" t="n">
@@ -18806,7 +18808,7 @@
         </is>
       </c>
       <c r="P41" s="20" t="n">
-        <v>7151</v>
+        <v>7170</v>
       </c>
       <c r="T41" s="5" t="n"/>
     </row>
@@ -18846,7 +18848,7 @@
         </is>
       </c>
       <c r="P43" s="20" t="n">
-        <v>16750</v>
+        <v>16769</v>
       </c>
       <c r="T43" s="5" t="n"/>
     </row>
@@ -18870,7 +18872,7 @@
         </is>
       </c>
       <c r="M45" s="20" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T45" s="5" t="n"/>
     </row>
@@ -24751,18 +24753,18 @@
         <v>2005</v>
       </c>
       <c r="O197" s="15" t="n">
-        <v>7.77</v>
+        <v>7.65</v>
       </c>
       <c r="P197" s="7" t="n">
-        <v>567</v>
+        <v>607</v>
       </c>
       <c r="Q197" s="7" t="inlineStr">
         <is>
-          <t>Ulsteinvik</t>
+          <t>Sortland</t>
         </is>
       </c>
       <c r="R197" s="16" t="n">
-        <v>4.03</v>
+        <v>18.02</v>
       </c>
       <c r="T197" s="5" t="n"/>
     </row>
@@ -25526,7 +25528,7 @@
         </is>
       </c>
       <c r="P211" s="20" t="n">
-        <v>8013</v>
+        <v>8053</v>
       </c>
       <c r="T211" s="5" t="n"/>
     </row>
@@ -26416,7 +26418,7 @@
         </is>
       </c>
       <c r="P231" s="20" t="n">
-        <v>15059</v>
+        <v>15099</v>
       </c>
       <c r="T231" s="5" t="n"/>
     </row>
@@ -29994,20 +29996,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F284:G285"/>
-    <mergeCell ref="P96:Q97"/>
-    <mergeCell ref="P143:Q144"/>
-    <mergeCell ref="P284:Q285"/>
-    <mergeCell ref="F143:G144"/>
     <mergeCell ref="F2:G3"/>
-    <mergeCell ref="P190:Q191"/>
     <mergeCell ref="P2:Q3"/>
     <mergeCell ref="F49:G50"/>
+    <mergeCell ref="P49:Q50"/>
+    <mergeCell ref="F96:G97"/>
+    <mergeCell ref="P96:Q97"/>
+    <mergeCell ref="F143:G144"/>
+    <mergeCell ref="P143:Q144"/>
     <mergeCell ref="F190:G191"/>
+    <mergeCell ref="P190:Q191"/>
     <mergeCell ref="F237:G238"/>
-    <mergeCell ref="P49:Q50"/>
     <mergeCell ref="P237:Q238"/>
-    <mergeCell ref="F96:G97"/>
+    <mergeCell ref="F284:G285"/>
+    <mergeCell ref="P284:Q285"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -30162,7 +30164,7 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>23024</v>
+        <v>23032</v>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
@@ -30190,7 +30192,7 @@
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>22883</v>
+        <v>22884</v>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
@@ -33071,25 +33073,25 @@
       </c>
       <c r="M63" s="7" t="inlineStr">
         <is>
-          <t>Ida Andrea Breigan</t>
+          <t>Marlen Aakre</t>
         </is>
       </c>
       <c r="N63" s="7" t="n">
-        <v>2004</v>
+        <v>1993</v>
       </c>
       <c r="O63" s="15" t="n">
-        <v>24.73</v>
+        <v>24.65</v>
       </c>
       <c r="P63" s="7" t="n">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="Q63" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Gøteborg/SWE</t>
         </is>
       </c>
       <c r="R63" s="16" t="n">
-        <v>16.06</v>
+        <v>16.07</v>
       </c>
       <c r="T63" s="5" t="n"/>
     </row>
@@ -33851,7 +33853,7 @@
         </is>
       </c>
       <c r="P77" s="20" t="n">
-        <v>11903</v>
+        <v>11910</v>
       </c>
       <c r="T77" s="5" t="n"/>
     </row>
@@ -34103,25 +34105,25 @@
       </c>
       <c r="M84" s="7" t="inlineStr">
         <is>
-          <t>Marlen Aakre</t>
+          <t>Ida Andrea Breigan</t>
         </is>
       </c>
       <c r="N84" s="7" t="n">
-        <v>1993</v>
+        <v>2004</v>
       </c>
       <c r="O84" s="15" t="n">
-        <v>24.74</v>
+        <v>24.73</v>
       </c>
       <c r="P84" s="7" t="n">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="Q84" s="7" t="inlineStr">
         <is>
-          <t>Oslo/Bi</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="R84" s="16" t="n">
-        <v>4.06</v>
+        <v>16.06</v>
       </c>
       <c r="T84" s="5" t="n"/>
     </row>
@@ -34873,7 +34875,7 @@
         </is>
       </c>
       <c r="P98" s="20" t="n">
-        <v>11121</v>
+        <v>11122</v>
       </c>
       <c r="T98" s="5" t="n"/>
     </row>
@@ -34913,7 +34915,7 @@
         </is>
       </c>
       <c r="P100" s="20" t="n">
-        <v>23024</v>
+        <v>23032</v>
       </c>
       <c r="T100" s="5" t="n"/>
     </row>
@@ -35982,18 +35984,18 @@
         <v>2005</v>
       </c>
       <c r="E127" s="15" t="n">
-        <v>47.4</v>
+        <v>47.48</v>
       </c>
       <c r="F127" s="7" t="n">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G127" s="7" t="inlineStr">
         <is>
-          <t>Mannheim/GER</t>
+          <t>Bottnaryd/SWE</t>
         </is>
       </c>
       <c r="H127" s="16" t="n">
-        <v>24.06</v>
+        <v>16.07</v>
       </c>
       <c r="J127" s="5" t="n"/>
       <c r="L127" s="14" t="inlineStr">
@@ -36058,7 +36060,7 @@
         </is>
       </c>
       <c r="F129" s="20" t="n">
-        <v>11867</v>
+        <v>11868</v>
       </c>
       <c r="J129" s="5" t="n"/>
       <c r="L129" s="19" t="inlineStr">
@@ -37124,7 +37126,7 @@
         </is>
       </c>
       <c r="F152" s="20" t="n">
-        <v>22883</v>
+        <v>22884</v>
       </c>
       <c r="J152" s="5" t="n"/>
       <c r="L152" s="19" t="inlineStr">
@@ -45897,20 +45899,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="P262:Q263"/>
-    <mergeCell ref="F210:G211"/>
     <mergeCell ref="F2:G3"/>
+    <mergeCell ref="P2:Q3"/>
     <mergeCell ref="F54:G55"/>
-    <mergeCell ref="P314:Q315"/>
-    <mergeCell ref="F314:G315"/>
     <mergeCell ref="P54:Q55"/>
-    <mergeCell ref="P2:Q3"/>
     <mergeCell ref="F106:G107"/>
+    <mergeCell ref="P106:Q107"/>
     <mergeCell ref="F158:G159"/>
     <mergeCell ref="P158:Q159"/>
+    <mergeCell ref="F210:G211"/>
     <mergeCell ref="P210:Q211"/>
-    <mergeCell ref="P106:Q107"/>
     <mergeCell ref="F262:G263"/>
+    <mergeCell ref="P262:Q263"/>
+    <mergeCell ref="F314:G315"/>
+    <mergeCell ref="P314:Q315"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -46341,11 +46343,11 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>(15/7)</t>
+          <t>(14/6)</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>8259</v>
+        <v>7890</v>
       </c>
       <c r="E16" s="4" t="inlineStr">
         <is>
@@ -59137,33 +59139,13 @@
         <v>21.01</v>
       </c>
       <c r="J314" s="5" t="n"/>
-      <c r="L314" s="14" t="inlineStr">
-        <is>
-          <t>60m</t>
-        </is>
-      </c>
-      <c r="M314" s="7" t="inlineStr">
-        <is>
-          <t>Maria Betten Lade</t>
-        </is>
-      </c>
-      <c r="N314" s="7" t="n">
-        <v>2009</v>
-      </c>
-      <c r="O314" s="15" t="n">
-        <v>9.49</v>
-      </c>
-      <c r="P314" s="7" t="n">
-        <v>369</v>
-      </c>
-      <c r="Q314" s="7" t="inlineStr">
-        <is>
-          <t>Stjørdal</t>
-        </is>
-      </c>
-      <c r="R314" s="16" t="n">
-        <v>21.06</v>
-      </c>
+      <c r="L314" s="14" t="n"/>
+      <c r="M314" s="7" t="n"/>
+      <c r="N314" s="7" t="n"/>
+      <c r="O314" s="7" t="n"/>
+      <c r="P314" s="7" t="n"/>
+      <c r="Q314" s="7" t="n"/>
+      <c r="R314" s="21" t="n"/>
       <c r="T314" s="5" t="n"/>
     </row>
     <row r="315" ht="13" customHeight="1">
@@ -59394,7 +59376,7 @@
         </is>
       </c>
       <c r="M323" s="20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O323" s="19" t="inlineStr">
         <is>
@@ -59402,7 +59384,7 @@
         </is>
       </c>
       <c r="P323" s="20" t="n">
-        <v>2773</v>
+        <v>2404</v>
       </c>
       <c r="T323" s="5" t="n"/>
     </row>
@@ -59434,7 +59416,7 @@
         </is>
       </c>
       <c r="M325" s="20" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O325" s="19" t="inlineStr">
         <is>
@@ -59442,7 +59424,7 @@
         </is>
       </c>
       <c r="P325" s="20" t="n">
-        <v>8259</v>
+        <v>7890</v>
       </c>
       <c r="T325" s="5" t="n"/>
     </row>
@@ -59466,7 +59448,7 @@
         </is>
       </c>
       <c r="M327" s="20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T327" s="5" t="n"/>
     </row>
@@ -59498,20 +59480,20 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F284:G285"/>
-    <mergeCell ref="P96:Q97"/>
-    <mergeCell ref="P143:Q144"/>
-    <mergeCell ref="P284:Q285"/>
-    <mergeCell ref="F143:G144"/>
     <mergeCell ref="F2:G3"/>
-    <mergeCell ref="P190:Q191"/>
     <mergeCell ref="P2:Q3"/>
     <mergeCell ref="F49:G50"/>
+    <mergeCell ref="P49:Q50"/>
+    <mergeCell ref="F96:G97"/>
+    <mergeCell ref="P96:Q97"/>
+    <mergeCell ref="F143:G144"/>
+    <mergeCell ref="P143:Q144"/>
     <mergeCell ref="F190:G191"/>
+    <mergeCell ref="P190:Q191"/>
     <mergeCell ref="F237:G238"/>
-    <mergeCell ref="P49:Q50"/>
     <mergeCell ref="P237:Q238"/>
-    <mergeCell ref="F96:G97"/>
+    <mergeCell ref="F284:G285"/>
+    <mergeCell ref="P284:Q285"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>